<commit_message>
added new code design for single options and nested options and getting preferred units function
</commit_message>
<xml_diff>
--- a/utils/excel_files/destination.xlsx
+++ b/utils/excel_files/destination.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navid\OneDrive\Desktop\MIT\cript-excel-uploader\utils\Excel File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navid\OneDrive\Desktop\MIT\cript-excel-uploader\utils\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D46C9D-7E94-4DBD-BD8E-30F1DD07E4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B202C2-B842-4471-8062-7B0550BC3502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D72C688-1DEF-4859-8406-CE6101F2A403}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Row 2 Value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Row 1 Value</t>
   </si>
@@ -402,7 +399,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,16 +414,17 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>